<commit_message>
2024 update 8 - update sprint categories.
</commit_message>
<xml_diff>
--- a/uploads/StartList_Amended.xlsx
+++ b/uploads/StartList_Amended.xlsx
@@ -3226,8 +3226,8 @@
   </sheetPr>
   <dimension ref="A1:O383"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A371" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K382" activeCellId="0" sqref="K382:K383"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A275" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D296" activeCellId="0" sqref="D296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14590,7 +14590,7 @@
         <v>98</v>
       </c>
       <c r="D296" s="2" t="s">
-        <v>149</v>
+        <v>23</v>
       </c>
       <c r="E296" s="5" t="n">
         <v>0.375</v>

</xml_diff>